<commit_message>
add test data and helpers
</commit_message>
<xml_diff>
--- a/tests/data/AciclovirLaskinData.xlsx
+++ b/tests/data/AciclovirLaskinData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svavil\Downloads\esqlabs\esqlabs.ParameterIdentification\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RudolfEngelke\Documents\RStudio.wd\OSPSuite.ParameterIdentification\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9B55CE-A577-4D9B-B97F-F0946B98A789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAC4A01-BC58-4B84-96F5-CBC045186375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD100792-66DE-42FA-AA26-60DC91D43834}"/>
+    <workbookView xWindow="13350" yWindow="1080" windowWidth="19580" windowHeight="18980" xr2:uid="{BD100792-66DE-42FA-AA26-60DC91D43834}"/>
   </bookViews>
   <sheets>
     <sheet name="Laskin 1982.Group A" sheetId="8" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -137,6 +137,7 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,8 +168,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FBF1C9A9-AE8C-48BC-98CF-4D21EF64E682}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -184,9 +185,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,7 +225,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -330,7 +331,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,7 +473,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -989,14 +990,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1237,21 +1236,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAB5050-D493-406E-92F7-9DBD52364DAC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E14CB4EF-58DD-43B7-9F24-675C988FD4B3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1276,9 +1274,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E14CB4EF-58DD-43B7-9F24-675C988FD4B3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAB5050-D493-406E-92F7-9DBD52364DAC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Resampling of dataset weights in PI for bootstrap method (#189)
* add bootstrap logic in PI

* add dataset classification logic

* add mapping weight extraction

* add weight updating functions

* add weight resampling logic (individuals data)

* fix bootstrap result dimension drop

* move observed data classification

* check activeBootstrapSeed NULL

* stop if obsVsSim/outputMapping length mismatch

* move inline messages to functions

* restore outputMappings state after bootstrap

* add test data and helpers

* test bootstrap using PI$estimateCI()
</commit_message>
<xml_diff>
--- a/tests/data/AciclovirLaskinData.xlsx
+++ b/tests/data/AciclovirLaskinData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\svavil\Downloads\esqlabs\esqlabs.ParameterIdentification\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RudolfEngelke\Documents\RStudio.wd\OSPSuite.ParameterIdentification\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9B55CE-A577-4D9B-B97F-F0946B98A789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAC4A01-BC58-4B84-96F5-CBC045186375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD100792-66DE-42FA-AA26-60DC91D43834}"/>
+    <workbookView xWindow="13350" yWindow="1080" windowWidth="19580" windowHeight="18980" xr2:uid="{BD100792-66DE-42FA-AA26-60DC91D43834}"/>
   </bookViews>
   <sheets>
     <sheet name="Laskin 1982.Group A" sheetId="8" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -137,6 +137,7 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,8 +168,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FBF1C9A9-AE8C-48BC-98CF-4D21EF64E682}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -184,9 +185,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,7 +225,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -330,7 +331,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,7 +473,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -989,14 +990,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1237,21 +1236,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAB5050-D493-406E-92F7-9DBD52364DAC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E14CB4EF-58DD-43B7-9F24-675C988FD4B3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1276,9 +1274,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E14CB4EF-58DD-43B7-9F24-675C988FD4B3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAB5050-D493-406E-92F7-9DBD52364DAC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>